<commit_message>
Doyle + LG_M50 Buildable - Cleanup
</commit_message>
<xml_diff>
--- a/src/Data/Chen_2020/Locations.xlsx
+++ b/src/Data/Chen_2020/Locations.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradyplanden/Documents/Git/LIBRA/src/Data/Chen_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A86DB446-3302-104A-B66C-A23C0673F35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0D250C-DF06-524E-B4AC-5A7A2824FD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="17540" xr2:uid="{E05F903E-98A3-7E4F-B01F-80C4791E9D97}"/>
+    <workbookView xWindow="640" yWindow="500" windowWidth="14080" windowHeight="17500" xr2:uid="{E05F903E-98A3-7E4F-B01F-80C4791E9D97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Neg</t>
   </si>
@@ -123,6 +123,9 @@
       </rPr>
       <t>1.73E-04</t>
     </r>
+  </si>
+  <si>
+    <t>Chen 2020</t>
   </si>
 </sst>
 </file>
@@ -489,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E03CD1-DAD7-E143-81E2-DB089F509024}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,79 +505,104 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>8.5199999999999997E-5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>1.2E-5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>7.5599999999999994E-5</v>
       </c>
-      <c r="D2" s="1">
-        <f>SUM(A2:C2)</f>
+      <c r="D3" s="1">
+        <f>SUM(A3:C3)</f>
         <v>1.728E-4</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <f>D2/6</f>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f>D3/6</f>
         <v>2.8799999999999999E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>0</v>
       </c>
-      <c r="B9" s="1">
-        <f>A2/2</f>
+      <c r="B10" s="1">
+        <f>A3/2</f>
         <v>4.2599999999999999E-5</v>
       </c>
-      <c r="C9" s="1">
-        <f>A2</f>
+      <c r="C10" s="1">
+        <f>A3</f>
         <v>8.5199999999999997E-5</v>
       </c>
-      <c r="D9" s="1">
-        <f>B2+A2</f>
+      <c r="D10" s="1">
+        <f>B3+A3</f>
         <v>9.7200000000000004E-5</v>
       </c>
-      <c r="E9" s="1">
-        <f>D9+(F9-D9)/2</f>
+      <c r="E10" s="1">
+        <f>D10+(F10-D10)/2</f>
         <v>1.35E-4</v>
       </c>
-      <c r="F9" s="1">
-        <f>D2</f>
+      <c r="F10" s="1">
+        <f>D3</f>
         <v>1.728E-4</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <f>0.0001728</f>
         <v>1.728E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F10" s="1">
-        <f>0.000173</f>
-        <v>1.73E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updt. Cell Data Struct / Benchmarking
</commit_message>
<xml_diff>
--- a/src/Data/Chen_2020/Locations.xlsx
+++ b/src/Data/Chen_2020/Locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradyplanden/Documents/Git/LIBRA/src/Data/Chen_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0D250C-DF06-524E-B4AC-5A7A2824FD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB64921-378F-004D-9854-7306270BAEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="500" windowWidth="14080" windowHeight="17500" xr2:uid="{E05F903E-98A3-7E4F-B01F-80C4791E9D97}"/>
+    <workbookView xWindow="680" yWindow="500" windowWidth="28120" windowHeight="17500" xr2:uid="{E05F903E-98A3-7E4F-B01F-80C4791E9D97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Neg</t>
   </si>
@@ -126,12 +126,21 @@
   </si>
   <si>
     <t>Chen 2020</t>
+  </si>
+  <si>
+    <t>Electrolyte Step Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Electrolyte </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000000E+00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -173,11 +182,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,23 +502,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E03CD1-DAD7-E143-81E2-DB089F509024}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -522,7 +533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>8.5199999999999997E-5</v>
       </c>
@@ -538,45 +549,61 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <f>D3/6</f>
-        <v>2.8799999999999999E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <f>D3/B7</f>
+        <v>3.4560000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>0</v>
       </c>
-      <c r="B10" s="1">
-        <f>A3/2</f>
-        <v>4.2599999999999999E-5</v>
-      </c>
-      <c r="C10" s="1">
-        <f>A3</f>
-        <v>8.5199999999999997E-5</v>
-      </c>
-      <c r="D10" s="1">
-        <f>B3+A3</f>
-        <v>9.7200000000000004E-5</v>
-      </c>
-      <c r="E10" s="1">
-        <f>D10+(F10-D10)/2</f>
-        <v>1.35E-4</v>
-      </c>
-      <c r="F10" s="1">
-        <f>D3</f>
+      <c r="B10" s="4">
+        <f>A10+$B$6</f>
+        <v>3.4560000000000001E-5</v>
+      </c>
+      <c r="C10" s="4">
+        <f>B10+$B$6</f>
+        <v>6.9120000000000002E-5</v>
+      </c>
+      <c r="D10" s="4">
+        <f>C10+$B$6</f>
+        <v>1.0368000000000001E-4</v>
+      </c>
+      <c r="E10" s="4">
+        <f>D10+$B$6</f>
+        <v>1.3824E-4</v>
+      </c>
+      <c r="F10" s="4">
+        <f>E10+$B$6</f>
         <v>1.728E-4</v>
       </c>
-      <c r="H10">
-        <f>0.0001728</f>
-        <v>1.728E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="4">
+        <f>F10+$B$6</f>
+        <v>2.0735999999999999E-4</v>
+      </c>
+      <c r="H10" s="4">
+        <f>G10+$B$6</f>
+        <v>2.4191999999999999E-4</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F11" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Benchmark Integration Commit #1
</commit_message>
<xml_diff>
--- a/src/Data/Chen_2020/Locations.xlsx
+++ b/src/Data/Chen_2020/Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradyplanden/Documents/Git/LIBRA/src/Data/Chen_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB64921-378F-004D-9854-7306270BAEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EF563C-B2B1-4C44-8EB9-151FE4215F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="28120" windowHeight="17500" xr2:uid="{E05F903E-98A3-7E4F-B01F-80C4791E9D97}"/>
+    <workbookView xWindow="640" yWindow="500" windowWidth="14080" windowHeight="17500" xr2:uid="{E05F903E-98A3-7E4F-B01F-80C4791E9D97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Neg</t>
   </si>
@@ -128,18 +128,28 @@
     <t>Chen 2020</t>
   </si>
   <si>
-    <t>Electrolyte Step Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Electrolyte </t>
+    <t>Electrolyte Neg Step Size</t>
+  </si>
+  <si>
+    <t>Electrolyte Pos Step Size</t>
+  </si>
+  <si>
+    <t>Electrolyte Sep Step Size</t>
+  </si>
+  <si>
+    <t>Number in Electrodes</t>
+  </si>
+  <si>
+    <t>Number in Seperator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000000E+00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -182,11 +192,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -502,16 +513,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E03CD1-DAD7-E143-81E2-DB089F509024}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -549,87 +562,122 @@
       </c>
       <c r="F3" s="1"/>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="1"/>
+    </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <f>D3/B7</f>
-        <v>3.4560000000000001E-5</v>
+        <f>A3/B9</f>
+        <v>2.8399999999999999E-5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <f>B3/B10</f>
+        <v>1.2E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>5</v>
+      <c r="B8" s="1">
+        <f>C3/B9</f>
+        <v>2.5199999999999999E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>0</v>
       </c>
-      <c r="B10" s="4">
-        <f>A10+$B$6</f>
-        <v>3.4560000000000001E-5</v>
-      </c>
-      <c r="C10" s="4">
-        <f>B10+$B$6</f>
-        <v>6.9120000000000002E-5</v>
-      </c>
-      <c r="D10" s="4">
-        <f>C10+$B$6</f>
-        <v>1.0368000000000001E-4</v>
-      </c>
-      <c r="E10" s="4">
-        <f>D10+$B$6</f>
-        <v>1.3824E-4</v>
-      </c>
-      <c r="F10" s="4">
-        <f>E10+$B$6</f>
-        <v>1.728E-4</v>
-      </c>
-      <c r="G10" s="4">
-        <f>F10+$B$6</f>
-        <v>2.0735999999999999E-4</v>
-      </c>
-      <c r="H10" s="4">
-        <f>G10+$B$6</f>
-        <v>2.4191999999999999E-4</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F11" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="B13" s="5">
+        <f t="shared" ref="B13:H13" si="0">A13+$B$6</f>
+        <v>2.8399999999999999E-5</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6799999999999998E-5</v>
+      </c>
+      <c r="D13" s="5">
+        <f>C13+B6</f>
+        <v>8.5199999999999997E-5</v>
+      </c>
+      <c r="E13" s="5">
+        <f>D13+B7</f>
+        <v>9.7200000000000004E-5</v>
+      </c>
+      <c r="F13" s="5">
+        <f>B8+E13</f>
+        <v>1.2239999999999999E-4</v>
+      </c>
+      <c r="G13" s="5">
+        <f>F13+B8</f>
+        <v>1.4759999999999998E-4</v>
+      </c>
+      <c r="H13" s="5">
+        <f>G13+B8</f>
+        <v>1.7279999999999997E-4</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F30" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>